<commit_message>
finish up work for today
</commit_message>
<xml_diff>
--- a/TODO/1-Saturday/Budget.xlsx
+++ b/TODO/1-Saturday/Budget.xlsx
@@ -17,20 +17,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t>Operation Budget</t>
   </si>
   <si>
-    <t>Category</t>
-  </si>
-  <si>
     <t>Quantity</t>
   </si>
   <si>
-    <t>Descriptoin</t>
-  </si>
-  <si>
     <t>Monthly Cost</t>
   </si>
   <si>
@@ -40,15 +34,9 @@
     <t>Rent</t>
   </si>
   <si>
-    <t>Internet</t>
-  </si>
-  <si>
     <t>Utilites</t>
   </si>
   <si>
-    <t>Phone</t>
-  </si>
-  <si>
     <t>Office supplies</t>
   </si>
   <si>
@@ -80,13 +68,76 @@
   </si>
   <si>
     <t>Cost</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Internet/Phone</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>tax</t>
+  </si>
+  <si>
+    <t>interest</t>
+  </si>
+  <si>
+    <t>net</t>
+  </si>
+  <si>
+    <t>EBIT</t>
+  </si>
+  <si>
+    <t>EBT</t>
+  </si>
+  <si>
+    <t>P &amp; L</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Unit cost</t>
+  </si>
+  <si>
+    <t>networking</t>
+  </si>
+  <si>
+    <t>phones</t>
+  </si>
+  <si>
+    <t>copier</t>
+  </si>
+  <si>
+    <t>desktop</t>
+  </si>
+  <si>
+    <t>server</t>
+  </si>
+  <si>
+    <t>Office equipment</t>
+  </si>
+  <si>
+    <t>Desk</t>
+  </si>
+  <si>
+    <t>Charis</t>
+  </si>
+  <si>
+    <t>cabinetts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,6 +149,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -117,7 +176,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -140,11 +199,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -153,6 +230,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -484,168 +585,403 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K11"/>
+  <dimension ref="B2:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F11" sqref="F11:J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="23.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="23.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="15.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="18" style="4" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="23.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" style="1" customWidth="1"/>
+    <col min="9" max="10" width="17.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" style="4" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="11"/>
+    </row>
+    <row r="3" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="4">
+        <v>985500</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="6">
+        <v>12000</v>
+      </c>
+      <c r="D4" s="6">
+        <f>C4*12</f>
+        <v>144000</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="6">
+        <v>10000</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="9">
+        <f>D11</f>
+        <v>847120</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1400</v>
+      </c>
+      <c r="D5" s="6">
+        <f>C5*12</f>
+        <v>16800</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="6">
+        <f>SUM(H12:H14)</f>
+        <v>50000</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="4">
+        <f>L3-L4</f>
+        <v>138380</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="6">
+        <v>360</v>
+      </c>
+      <c r="D6" s="6">
+        <f>C6*12</f>
+        <v>4320</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="6">
+        <f>SUM(H15:H19)</f>
+        <v>8750</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6">
+        <v>2000</v>
+      </c>
+      <c r="D7" s="6">
+        <f>C7*12</f>
+        <v>24000</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="G7" s="6">
+        <v>20000</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="4">
+        <f>L5-L6</f>
+        <v>138380</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="6">
+        <v>5000</v>
+      </c>
+      <c r="D8" s="6">
+        <f>C8*12</f>
+        <v>60000</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="6">
+        <v>5000</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="10">
+        <f>L7*0.39</f>
+        <v>53968.200000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="6">
+        <f>D9/12</f>
+        <v>49583.333333333336</v>
+      </c>
+      <c r="D9" s="6">
+        <v>595000</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="8">
+        <f>SUM(G4:G8)</f>
+        <v>93750</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9" s="4">
+        <f>L7-L8</f>
+        <v>84411.799999999988</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="6">
+        <v>250</v>
+      </c>
+      <c r="D10" s="6">
+        <f>C10*12</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="8">
+        <f>SUM(C4:C10)</f>
+        <v>70593.333333333343</v>
+      </c>
+      <c r="D11" s="8">
+        <f>SUM(D4:D10)</f>
+        <v>847120</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2" t="s">
+    </row>
+    <row r="12" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="6">
+        <f>I12*J12</f>
+        <v>22000</v>
+      </c>
+      <c r="I12" s="6">
+        <v>2000</v>
+      </c>
+      <c r="J12" s="6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="6">
+        <f>I13*J13</f>
+        <v>24000</v>
+      </c>
+      <c r="I13" s="6">
+        <v>8000</v>
+      </c>
+      <c r="J13" s="6">
         <v>3</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="2" t="s">
+    </row>
+    <row r="14" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="6">
+        <f>I14*J14</f>
+        <v>4000</v>
+      </c>
+      <c r="I14" s="6">
+        <v>4000</v>
+      </c>
+      <c r="J14" s="6">
         <v>1</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="H4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+    </row>
+    <row r="15" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" s="6">
+        <f>I15*J15</f>
+        <v>4500</v>
+      </c>
+      <c r="I15" s="6">
+        <v>500</v>
+      </c>
+      <c r="J15" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16" s="6">
+        <f>I16*J16</f>
+        <v>1350</v>
+      </c>
+      <c r="I16" s="6">
+        <v>150</v>
+      </c>
+      <c r="J16" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="6:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H17" s="6">
+        <f>I17*J17</f>
+        <v>800</v>
+      </c>
+      <c r="I17" s="6">
+        <v>100</v>
+      </c>
+      <c r="J17" s="6">
         <v>8</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="H5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-    </row>
-    <row r="6" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="H6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-    </row>
-    <row r="7" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="H7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-    </row>
-    <row r="8" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="H8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-    </row>
-    <row r="9" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
+    </row>
+    <row r="18" spans="6:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" s="6">
+        <f>I18*J18</f>
+        <v>1100</v>
+      </c>
+      <c r="I18" s="6">
+        <v>100</v>
+      </c>
+      <c r="J18" s="6">
         <v>11</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
+    </row>
+    <row r="19" spans="6:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19" s="6">
+        <f>I19*J19</f>
+        <v>1000</v>
+      </c>
+      <c r="I19" s="6">
+        <v>1000</v>
+      </c>
+      <c r="J19" s="6">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="K2:L2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
fixing stuff and working on financials
</commit_message>
<xml_diff>
--- a/TODO/1-Saturday/Budget.xlsx
+++ b/TODO/1-Saturday/Budget.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="255" windowWidth="20250" windowHeight="9705"/>
+    <workbookView xWindow="480" yWindow="255" windowWidth="19320" windowHeight="9705"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -587,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11:J19"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -842,7 +842,7 @@
         <v>32</v>
       </c>
       <c r="H12" s="6">
-        <f>I12*J12</f>
+        <f t="shared" ref="H12:H19" si="0">I12*J12</f>
         <v>22000</v>
       </c>
       <c r="I12" s="6">
@@ -860,7 +860,7 @@
         <v>33</v>
       </c>
       <c r="H13" s="6">
-        <f>I13*J13</f>
+        <f t="shared" si="0"/>
         <v>24000</v>
       </c>
       <c r="I13" s="6">
@@ -878,7 +878,7 @@
         <v>29</v>
       </c>
       <c r="H14" s="6">
-        <f>I14*J14</f>
+        <f t="shared" si="0"/>
         <v>4000</v>
       </c>
       <c r="I14" s="6">
@@ -896,7 +896,7 @@
         <v>35</v>
       </c>
       <c r="H15" s="6">
-        <f>I15*J15</f>
+        <f t="shared" si="0"/>
         <v>4500</v>
       </c>
       <c r="I15" s="6">
@@ -914,7 +914,7 @@
         <v>36</v>
       </c>
       <c r="H16" s="6">
-        <f>I16*J16</f>
+        <f t="shared" si="0"/>
         <v>1350</v>
       </c>
       <c r="I16" s="6">
@@ -932,7 +932,7 @@
         <v>37</v>
       </c>
       <c r="H17" s="6">
-        <f>I17*J17</f>
+        <f t="shared" si="0"/>
         <v>800</v>
       </c>
       <c r="I17" s="6">
@@ -950,7 +950,7 @@
         <v>30</v>
       </c>
       <c r="H18" s="6">
-        <f>I18*J18</f>
+        <f t="shared" si="0"/>
         <v>1100</v>
       </c>
       <c r="I18" s="6">
@@ -968,7 +968,7 @@
         <v>31</v>
       </c>
       <c r="H19" s="6">
-        <f>I19*J19</f>
+        <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="I19" s="6">

</xml_diff>